<commit_message>
7 segment display encoded
</commit_message>
<xml_diff>
--- a/Port mapping.xlsx
+++ b/Port mapping.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andb7\MPLABXProjects\SerialCop4P\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EEADBCB-B3DE-4251-B437-462015838B68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDF3CFE-21B4-44FC-A104-BB562E8813D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9C70A16A-12F0-491F-9F17-839333B215EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Disp7seg" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="92">
   <si>
     <t>CON4 – DIGITAL:</t>
   </si>
@@ -249,13 +250,70 @@
   </si>
   <si>
     <t>OUT</t>
+  </si>
+  <si>
+    <t>https://www.nutsvolts.com/magazine/article/using-seven-segment-displays-part-1</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>DISP</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>-a-</t>
+  </si>
+  <si>
+    <t>-g-</t>
+  </si>
+  <si>
+    <t>-d-</t>
+  </si>
+  <si>
+    <t>static const unsigned char display7s[] = {</t>
+  </si>
+  <si>
+    <t>}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,8 +337,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI Symbol"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,8 +357,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -368,11 +438,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -394,6 +538,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,7 +895,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="D7" sqref="D7:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,4 +1672,797 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9A07F8-9D92-46D6-9163-4A1A99EBEAC0}">
+  <dimension ref="A1:V19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:V18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1</v>
+      </c>
+      <c r="D3" s="15">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="20">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="array" ref="I3">SUM(A3:G3*A$19:G$19)</f>
+        <v>126</v>
+      </c>
+      <c r="J3" s="25" t="str">
+        <f>"0x" &amp;DEC2HEX(I3) &amp;","</f>
+        <v>0x7E,</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="23"/>
+      <c r="O3" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="P3" s="23"/>
+    </row>
+    <row r="4" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17">
+        <v>1</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="21">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f t="array" ref="I4">SUM(A4:G4*A$19:G$19)</f>
+        <v>48</v>
+      </c>
+      <c r="J4" s="25" t="str">
+        <f t="shared" ref="J4:J17" si="0">"0x" &amp;DEC2HEX(I4) &amp;","</f>
+        <v>0x30,</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" s="23"/>
+      <c r="P4" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>1</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17">
+        <v>1</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17">
+        <v>1</v>
+      </c>
+      <c r="H5" s="21">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <f t="array" ref="I5">SUM(A5:G5*A$19:G$19)</f>
+        <v>109</v>
+      </c>
+      <c r="J5" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x6D,</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="O5" s="23"/>
+      <c r="P5" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>1</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1</v>
+      </c>
+      <c r="C6" s="17">
+        <v>1</v>
+      </c>
+      <c r="D6" s="17">
+        <v>1</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17">
+        <v>1</v>
+      </c>
+      <c r="H6" s="21">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <f t="array" ref="I6">SUM(A6:G6*A$19:G$19)</f>
+        <v>121</v>
+      </c>
+      <c r="J6" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x79,</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6" s="23"/>
+      <c r="P6" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17">
+        <v>1</v>
+      </c>
+      <c r="C7" s="17">
+        <v>1</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17">
+        <v>1</v>
+      </c>
+      <c r="G7" s="17">
+        <v>1</v>
+      </c>
+      <c r="H7" s="21">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <f t="array" ref="I7">SUM(A7:G7*A$19:G$19)</f>
+        <v>51</v>
+      </c>
+      <c r="J7" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x33,</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7" s="23"/>
+      <c r="O7" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="P7" s="23"/>
+    </row>
+    <row r="8" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>1</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17">
+        <v>1</v>
+      </c>
+      <c r="D8" s="17">
+        <v>1</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17">
+        <v>1</v>
+      </c>
+      <c r="G8" s="17">
+        <v>1</v>
+      </c>
+      <c r="H8" s="21">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <f t="array" ref="I8">SUM(A8:G8*A$19:G$19)</f>
+        <v>91</v>
+      </c>
+      <c r="J8" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x5B,</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="O8" s="23"/>
+      <c r="P8" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>1</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17">
+        <v>1</v>
+      </c>
+      <c r="D9" s="17">
+        <v>1</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="17">
+        <v>1</v>
+      </c>
+      <c r="G9" s="17">
+        <v>1</v>
+      </c>
+      <c r="H9" s="21">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <f t="array" ref="I9">SUM(A9:G9*A$19:G$19)</f>
+        <v>95</v>
+      </c>
+      <c r="J9" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x5F,</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="O9" s="23"/>
+      <c r="P9" s="24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>1</v>
+      </c>
+      <c r="B10" s="19">
+        <v>1</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="22">
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <f t="array" ref="I10">SUM(A10:G10*A$19:G$19)</f>
+        <v>112</v>
+      </c>
+      <c r="J10" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x70,</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="O10" s="23"/>
+      <c r="P10" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15">
+        <v>1</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15">
+        <v>1</v>
+      </c>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="15">
+        <v>1</v>
+      </c>
+      <c r="H11" s="20">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <f t="array" ref="I11">SUM(A11:G11*A$19:G$19)</f>
+        <v>127</v>
+      </c>
+      <c r="J11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x7F,</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="23"/>
+      <c r="O11" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="P11" s="23"/>
+    </row>
+    <row r="12" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>1</v>
+      </c>
+      <c r="B12" s="17">
+        <v>1</v>
+      </c>
+      <c r="C12" s="17">
+        <v>1</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17">
+        <v>1</v>
+      </c>
+      <c r="G12" s="17">
+        <v>1</v>
+      </c>
+      <c r="H12" s="21">
+        <v>9</v>
+      </c>
+      <c r="I12">
+        <f t="array" ref="I12">SUM(A12:G12*A$19:G$19)</f>
+        <v>115</v>
+      </c>
+      <c r="J12" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x73,</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>1</v>
+      </c>
+      <c r="B13" s="17">
+        <v>1</v>
+      </c>
+      <c r="C13" s="17">
+        <v>1</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17">
+        <v>1</v>
+      </c>
+      <c r="F13" s="17">
+        <v>1</v>
+      </c>
+      <c r="G13" s="17">
+        <v>1</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13">
+        <f t="array" ref="I13">SUM(A13:G13*A$19:G$19)</f>
+        <v>119</v>
+      </c>
+      <c r="J13" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x77,</v>
+      </c>
+      <c r="L13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17">
+        <v>1</v>
+      </c>
+      <c r="D14" s="17">
+        <v>1</v>
+      </c>
+      <c r="E14" s="17">
+        <v>1</v>
+      </c>
+      <c r="F14" s="17">
+        <v>1</v>
+      </c>
+      <c r="G14" s="17">
+        <v>1</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14">
+        <f t="array" ref="I14">SUM(A14:G14*A$19:G$19)</f>
+        <v>31</v>
+      </c>
+      <c r="J14" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x1F,</v>
+      </c>
+      <c r="M14" t="str">
+        <f>J3</f>
+        <v>0x7E,</v>
+      </c>
+      <c r="N14" t="str">
+        <f>J4</f>
+        <v>0x30,</v>
+      </c>
+      <c r="O14" t="str">
+        <f>J5</f>
+        <v>0x6D,</v>
+      </c>
+      <c r="P14" t="str">
+        <f>J6</f>
+        <v>0x79,</v>
+      </c>
+      <c r="R14" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="S14" s="13">
+        <f>H3</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="13">
+        <f>H4</f>
+        <v>1</v>
+      </c>
+      <c r="U14" s="13">
+        <f>H5</f>
+        <v>2</v>
+      </c>
+      <c r="V14" s="13">
+        <f>H6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>1</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17">
+        <v>1</v>
+      </c>
+      <c r="E15" s="17">
+        <v>1</v>
+      </c>
+      <c r="F15" s="17">
+        <v>1</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I15">
+        <f t="array" ref="I15">SUM(A15:G15*A$19:G$19)</f>
+        <v>78</v>
+      </c>
+      <c r="J15" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x4E,</v>
+      </c>
+      <c r="M15" t="str">
+        <f>J7</f>
+        <v>0x33,</v>
+      </c>
+      <c r="N15" t="str">
+        <f>J8</f>
+        <v>0x5B,</v>
+      </c>
+      <c r="O15" t="str">
+        <f>J9</f>
+        <v>0x5F,</v>
+      </c>
+      <c r="P15" t="str">
+        <f>J10</f>
+        <v>0x70,</v>
+      </c>
+      <c r="R15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="S15" s="13">
+        <f>H7</f>
+        <v>4</v>
+      </c>
+      <c r="T15" s="13">
+        <f>H8</f>
+        <v>5</v>
+      </c>
+      <c r="U15" s="13">
+        <f>H9</f>
+        <v>6</v>
+      </c>
+      <c r="V15" s="13">
+        <f>H10</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17">
+        <v>1</v>
+      </c>
+      <c r="C16" s="17">
+        <v>1</v>
+      </c>
+      <c r="D16" s="17">
+        <v>1</v>
+      </c>
+      <c r="E16" s="17">
+        <v>1</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17">
+        <v>1</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16">
+        <f t="array" ref="I16">SUM(A16:G16*A$19:G$19)</f>
+        <v>61</v>
+      </c>
+      <c r="J16" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x3D,</v>
+      </c>
+      <c r="M16" t="str">
+        <f>J11</f>
+        <v>0x7F,</v>
+      </c>
+      <c r="N16" t="str">
+        <f>J12</f>
+        <v>0x73,</v>
+      </c>
+      <c r="O16" t="str">
+        <f>J13</f>
+        <v>0x77,</v>
+      </c>
+      <c r="P16" t="str">
+        <f>J14</f>
+        <v>0x1F,</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="S16" s="13">
+        <f>H11</f>
+        <v>8</v>
+      </c>
+      <c r="T16" s="13">
+        <f>H12</f>
+        <v>9</v>
+      </c>
+      <c r="U16" s="13" t="str">
+        <f>H13</f>
+        <v>A</v>
+      </c>
+      <c r="V16" s="13" t="str">
+        <f>H14</f>
+        <v>b</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <v>1</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="17">
+        <v>1</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17">
+        <f t="array" ref="I17">SUM(A17:G17*A$19:G$19)</f>
+        <v>79</v>
+      </c>
+      <c r="J17" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0x4F,</v>
+      </c>
+      <c r="M17" t="str">
+        <f>J15</f>
+        <v>0x4E,</v>
+      </c>
+      <c r="N17" t="str">
+        <f>J16</f>
+        <v>0x3D,</v>
+      </c>
+      <c r="O17" t="str">
+        <f>J17</f>
+        <v>0x4F,</v>
+      </c>
+      <c r="P17" t="str">
+        <f>J18</f>
+        <v>0x47</v>
+      </c>
+      <c r="R17" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="S17" s="13" t="str">
+        <f>H15</f>
+        <v>C</v>
+      </c>
+      <c r="T17" s="13" t="str">
+        <f>H16</f>
+        <v>d</v>
+      </c>
+      <c r="U17" s="13" t="str">
+        <f>H17</f>
+        <v>E</v>
+      </c>
+      <c r="V17" s="13" t="str">
+        <f>H18</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19">
+        <v>1</v>
+      </c>
+      <c r="F18" s="19">
+        <v>1</v>
+      </c>
+      <c r="G18" s="19">
+        <v>1</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18">
+        <f t="array" ref="I18">SUM(A18:G18*A$19:G$19)</f>
+        <v>71</v>
+      </c>
+      <c r="J18" s="25" t="str">
+        <f t="shared" ref="J4:J18" si="1">"0x" &amp;DEC2HEX(I18)</f>
+        <v>0x47</v>
+      </c>
+      <c r="L18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <f t="shared" ref="A19:E19" si="2">B19*2</f>
+        <v>64</v>
+      </c>
+      <c r="B19" s="13">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="C19" s="13">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D19" s="13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F19" s="13">
+        <f>G19*2</f>
+        <v>2</v>
+      </c>
+      <c r="G19" s="13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="I12 I3:I11" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>